<commit_message>
Add style of delivery to upper level.
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Projects/100 Behaviour Change/BCIO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775F92DD-7071-314C-97D4-72F44A13D7EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCEC2E7-0272-F244-BB3A-641C1CCBA4CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18620" yWindow="460" windowWidth="18580" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClassDefs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="175">
   <si>
     <t>Definition</t>
   </si>
@@ -300,9 +300,6 @@
     <t xml:space="preserve">Research study (SEPIO)/Process </t>
   </si>
   <si>
-    <t>Need to explain what we mean by positive and negative. Needs examples.</t>
-  </si>
-  <si>
     <t>Intervention outcome</t>
   </si>
   <si>
@@ -354,9 +351,6 @@
     <t>Parent class/ BFO class</t>
   </si>
   <si>
-    <t>Elaboration</t>
-  </si>
-  <si>
     <t>An intervention evaluation study of a BCI scenario.</t>
   </si>
   <si>
@@ -538,6 +532,24 @@
   </si>
   <si>
     <t>Environmental system (ENVO)/Continuant</t>
+  </si>
+  <si>
+    <t>Examples of interventions are putting health warnings on cigarette packets, providing free stop smoking services and banning smoking in public places.</t>
+  </si>
+  <si>
+    <t>Behaviour change intervention style of delivery (BCI style of delivery)</t>
+  </si>
+  <si>
+    <t>An attribute of a BCI delivery that encompasses the characteristics of how a BCI is communicated.</t>
+  </si>
+  <si>
+    <t>An example is cold and distant vs. warm and accepting.</t>
+  </si>
+  <si>
+    <t>BCIO:044000</t>
+  </si>
+  <si>
+    <t>Examples</t>
   </si>
 </sst>
 </file>
@@ -934,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -956,19 +968,19 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>174</v>
       </c>
       <c r="M1" s="9"/>
       <c r="N1" s="4"/>
@@ -977,7 +989,7 @@
     </row>
     <row r="2" spans="1:17" s="13" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>2</v>
@@ -986,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1005,7 +1017,7 @@
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -1034,7 +1046,7 @@
     </row>
     <row r="4" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -1059,7 +1071,7 @@
     </row>
     <row r="5" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
@@ -1068,7 +1080,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>15</v>
@@ -1084,7 +1096,7 @@
     </row>
     <row r="6" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>16</v>
@@ -1107,7 +1119,7 @@
     </row>
     <row r="7" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
@@ -1132,7 +1144,7 @@
     </row>
     <row r="8" spans="1:17" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>22</v>
@@ -1157,16 +1169,16 @@
     </row>
     <row r="9" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>27</v>
@@ -1182,16 +1194,16 @@
     </row>
     <row r="10" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1205,7 +1217,7 @@
     </row>
     <row r="11" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>29</v>
@@ -1214,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>31</v>
@@ -1230,16 +1242,16 @@
     </row>
     <row r="12" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1253,7 +1265,7 @@
     </row>
     <row r="13" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>33</v>
@@ -1276,7 +1288,7 @@
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>36</v>
@@ -1285,7 +1297,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1313,7 +1325,7 @@
     </row>
     <row r="16" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>38</v>
@@ -1336,7 +1348,7 @@
     </row>
     <row r="17" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>41</v>
@@ -1359,7 +1371,7 @@
     </row>
     <row r="18" spans="1:17" s="3" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>43</v>
@@ -1387,7 +1399,7 @@
     </row>
     <row r="19" spans="1:17" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>47</v>
@@ -1396,7 +1408,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1413,7 +1425,7 @@
     </row>
     <row r="20" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>49</v>
@@ -1422,7 +1434,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1436,10 +1448,10 @@
     </row>
     <row r="21" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>51</v>
@@ -1459,7 +1471,7 @@
     </row>
     <row r="22" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>53</v>
@@ -1482,7 +1494,7 @@
     </row>
     <row r="23" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>56</v>
@@ -1504,7 +1516,7 @@
     </row>
     <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>59</v>
@@ -1528,7 +1540,7 @@
     </row>
     <row r="25" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>62</v>
@@ -1537,7 +1549,7 @@
         <v>63</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>64</v>
@@ -1552,7 +1564,7 @@
     </row>
     <row r="26" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>65</v>
@@ -1561,7 +1573,7 @@
         <v>66</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1574,16 +1586,16 @@
     </row>
     <row r="27" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>68</v>
@@ -1598,16 +1610,16 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>69</v>
@@ -1615,210 +1627,227 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="E39" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fix to definition of study plan
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B741D4-9A61-2149-BFE8-A526FDDBB002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9F2858-2EA1-374F-9163-9355C5A40894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>Behaviour change intervention evaluation study plan (BCI evaluation study plan)</t>
   </si>
   <si>
-    <t>A plan specification for a BCI evaluation study.</t>
-  </si>
-  <si>
     <t>Behaviour change intervention evaluation study risk of bias or error (BCI study risk of bias or error)</t>
   </si>
   <si>
@@ -547,6 +544,9 @@
   </si>
   <si>
     <t>An attribute of BCI delivery that encompasses the characteristics of how BCI content is communicated.</t>
+  </si>
+  <si>
+    <t>A plan for a BCI evaluation study.</t>
   </si>
 </sst>
 </file>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -965,19 +965,19 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M1" s="9"/>
       <c r="N1" s="4"/>
@@ -986,7 +986,7 @@
     </row>
     <row r="2" spans="1:17" s="13" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>2</v>
@@ -995,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="4" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -1068,16 +1068,16 @@
     </row>
     <row r="5" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1093,13 +1093,13 @@
     </row>
     <row r="6" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>11</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="7" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -1128,7 +1128,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="8" spans="1:17" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
@@ -1166,16 +1166,16 @@
     </row>
     <row r="9" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>24</v>
@@ -1191,16 +1191,16 @@
     </row>
     <row r="10" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="11" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -1223,7 +1223,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>28</v>
@@ -1239,16 +1239,16 @@
     </row>
     <row r="12" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1262,16 +1262,16 @@
     </row>
     <row r="13" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1285,16 +1285,16 @@
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1322,16 +1322,16 @@
     </row>
     <row r="16" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1345,13 +1345,13 @@
     </row>
     <row r="17" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>18</v>
@@ -1368,19 +1368,19 @@
     </row>
     <row r="18" spans="1:17" s="3" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1396,16 +1396,16 @@
     </row>
     <row r="19" spans="1:17" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1422,16 +1422,16 @@
     </row>
     <row r="20" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1445,16 +1445,16 @@
     </row>
     <row r="21" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1468,16 +1468,16 @@
     </row>
     <row r="22" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1491,16 +1491,16 @@
     </row>
     <row r="23" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1513,19 +1513,19 @@
     </row>
     <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1537,19 +1537,19 @@
     </row>
     <row r="25" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1561,16 +1561,16 @@
     </row>
     <row r="26" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1583,19 +1583,19 @@
     </row>
     <row r="27" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1607,78 +1607,78 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>11</v>
@@ -1686,165 +1686,165 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Capitalisation and change to human behaviour
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\OneDrive\Documents\GitHub\ontologies\Upper Level BCIO\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C6ED9F-8897-417B-B2FA-09F7E49A2DAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94412A76-9D7F-7543-9D12-8F23C5EC9471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11720" yWindow="-21140" windowWidth="25600" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -55,15 +55,9 @@
     <t>BCIO:003000</t>
   </si>
   <si>
-    <t>Behaviour change intervention (BCI)</t>
-  </si>
-  <si>
     <t>An intervention that has the aim of influencing human behaviour.</t>
   </si>
   <si>
-    <t xml:space="preserve">Intervention/Process </t>
-  </si>
-  <si>
     <t>Involves use of products, services, activities, rules or environmental objects.</t>
   </si>
   <si>
@@ -73,261 +67,147 @@
     <t>BCIO:016000</t>
   </si>
   <si>
-    <t>Behaviour change intervention comparison evaluation study (BCI comparison evaluation study)</t>
-  </si>
-  <si>
     <t xml:space="preserve">A BCI evaluation study that involves comparison between two or more BCI scenarios to produce one or more BCI effect estimates. </t>
   </si>
   <si>
-    <t xml:space="preserve">Behaviour change intervention evaluation study/Process </t>
-  </si>
-  <si>
     <t>Comparison involves identifying differences between the entities in the scenarios.</t>
   </si>
   <si>
     <t>BCIO:007000</t>
   </si>
   <si>
-    <t>Behaviour change intervention content (BCI content)</t>
-  </si>
-  <si>
     <t>A planned process that is part of a BCI and is intended to be causally active in influencing the outcome behaviour.</t>
   </si>
   <si>
-    <t>Planned process (OBI)/Process</t>
-  </si>
-  <si>
     <t xml:space="preserve">Consists of BCTs that can be classified using a BCT taxonomy. </t>
   </si>
   <si>
     <t>BCIO:005000</t>
   </si>
   <si>
-    <t>Behaviour change intervention context (BCI context)</t>
-  </si>
-  <si>
     <t>An aggregate of entities that are not dependent on the intervention but may influence the effect of a BCI on its outcome behaviour.</t>
   </si>
   <si>
-    <t>Object aggregate/Object aggregate</t>
-  </si>
-  <si>
     <t>Includes as part BCI population and BCI setting. Use of the word ‘may’ conveys a non-zero probability given available information.</t>
   </si>
   <si>
     <t>BCIO:008000</t>
   </si>
   <si>
-    <t>Behaviour change intervention delivery (BCI delivery)</t>
-  </si>
-  <si>
-    <t>A part of a BCI that is the process by which BCI content is delivered.</t>
-  </si>
-  <si>
     <t>BCIO:022000</t>
   </si>
   <si>
-    <t>Behaviour change intervention dose (BCI dose)</t>
-  </si>
-  <si>
     <t>An attribute of BCI content that is its amount or intensity.</t>
   </si>
   <si>
-    <t>Process attribute/Process</t>
-  </si>
-  <si>
     <t>This is a disjunctive class that is not currently fully defined because specific BCI content instances may vary in intensity and amount in different ways.</t>
   </si>
   <si>
     <t>BCIO:017000</t>
   </si>
   <si>
-    <t>Behaviour change intervention effect estimate (BCI effect estimate)</t>
-  </si>
-  <si>
     <t xml:space="preserve">A BCI evaluation finding that characterises the difference between BCI outcome estimates of two BCI scenarios. </t>
   </si>
   <si>
-    <t>BCI evaluation finding/Generically dependent continuant</t>
-  </si>
-  <si>
     <t>This includes the following subclasses: 1) BCI effect estimate type -the type of statistic used to represent the difference (e.g. odds ratio, mean difference), 2) BCI effect estimate value – the datum that represents the difference (e.g. 1.35), 3)  BCI effect estimate uncertainty type – the type of statistic used to represent the range of uncertainty of the value (e.g. 95% confidence interval see STATO), and 4) the BCI effect estimate uncertainty value  - the datum representing the uncertainty (e.g. 1.20-1.55).</t>
   </si>
   <si>
     <t>BCIO:013000</t>
   </si>
   <si>
-    <t>Behaviour change intervention engagement (BCI engagement)</t>
-  </si>
-  <si>
     <t>Individual human activity that enables a BCI to influence the outcome behaviour.</t>
   </si>
   <si>
-    <t xml:space="preserve">Individual human activity/Process </t>
-  </si>
-  <si>
     <t>Includes mental activities and behaviours.</t>
   </si>
   <si>
     <t>BCIO:023000</t>
   </si>
   <si>
-    <t>Behaviour change intervention evaluation finding (BCI evaluation finding)</t>
-  </si>
-  <si>
     <t>An evaluation finding that is the output of a BCI evaluation study.</t>
   </si>
   <si>
-    <t xml:space="preserve">Evaluation finding/Process </t>
-  </si>
-  <si>
     <t>BCIO:021000</t>
   </si>
   <si>
-    <t>Behaviour change intervention evaluation report (BCI evaluation report)</t>
-  </si>
-  <si>
     <t>A report that is a description of a BCI evaluation study.</t>
   </si>
   <si>
-    <t xml:space="preserve">Report (IAO)/Generically dependent continuant </t>
-  </si>
-  <si>
     <t>Includes entities that stand in direct relation to the study e.g. authors, findings, funding, aims.</t>
   </si>
   <si>
     <t>BCIO:018000</t>
   </si>
   <si>
-    <t>Behaviour change intervention evaluation study (BCI evaluation study)</t>
-  </si>
-  <si>
     <t>An intervention evaluation study of a BCI scenario.</t>
   </si>
   <si>
-    <t xml:space="preserve">Intervention evaluation study/Process </t>
-  </si>
-  <si>
     <t>BCIO:024000</t>
   </si>
   <si>
-    <t>Behaviour change intervention evaluation study plan (BCI evaluation study plan)</t>
-  </si>
-  <si>
     <t>A plan for a BCI evaluation study.</t>
   </si>
   <si>
-    <t>Plan (OBI)/Generically dependent continuant</t>
-  </si>
-  <si>
     <t>BCIO:020000</t>
   </si>
   <si>
-    <t>Behaviour change intervention evaluation study risk of bias or error (BCI study risk of bias or error)</t>
-  </si>
-  <si>
     <t>An information content entity that is about the likelihood of the BCI evaluation finding misrepresenting the outcome behaviour.</t>
   </si>
   <si>
-    <t>Information content entity (IAO)/Generically dependent continuant</t>
-  </si>
-  <si>
     <t>BCIO:006000</t>
   </si>
   <si>
-    <t>Behaviour change intervention mechanism of action (BCI mechanism of action)</t>
-  </si>
-  <si>
     <t xml:space="preserve">A process that is causally active in the relationship between a BCI and its outcome behaviour. </t>
   </si>
   <si>
-    <t xml:space="preserve">Process/Process </t>
-  </si>
-  <si>
     <t>BCIO:011000</t>
   </si>
   <si>
-    <t>Behaviour change intervention mode of delivery (BCI mode of delivery)</t>
-  </si>
-  <si>
     <t>An attribute of a BCI delivery that is the physical or informational medium through which a BCI is provided.</t>
   </si>
   <si>
     <t>BCIO:025000</t>
   </si>
   <si>
-    <t>Behaviour change intervention outcome estimate (BCI outcome estimate)</t>
-  </si>
-  <si>
     <t>A BCI evaluation finding that is about an outcome behaviour.</t>
   </si>
   <si>
-    <t>Behaviour change intervention evaluation finding/Generically dependent continuant</t>
-  </si>
-  <si>
     <t>This includes as subclasses 1) type of outcome estimate (e.g. mean, percentage), 2) value of outcome estimate (e.g. 1.5 cigs per day, 23%), 3) uncertainty estimate type (e.g. 95% CI), and 4) uncertainty estimate value (e.g. 12.0%-45.0%).</t>
   </si>
   <si>
     <t>BCIO:026000</t>
   </si>
   <si>
-    <t>Behaviour change intervention physical setting (BCI physical setting)</t>
-  </si>
-  <si>
     <t>A physical environment in which a BCI is delivered.</t>
   </si>
   <si>
-    <t>Environmental system (ENVO)/Continuant</t>
-  </si>
-  <si>
     <t>BCIO:015000</t>
   </si>
   <si>
-    <t>Behaviour change intervention population (BCI population)</t>
-  </si>
-  <si>
     <t xml:space="preserve">An aggregate of people who are exposed to a BCI. </t>
   </si>
   <si>
-    <t xml:space="preserve">Human population/Object aggregate </t>
-  </si>
-  <si>
     <t>BCIO:027000</t>
   </si>
   <si>
-    <t>Behaviour change intervention scenario report (BCI scenario report)</t>
-  </si>
-  <si>
     <t>A report that describes a BCI scenario.</t>
   </si>
   <si>
-    <t>Report (IAO)/Generically dependent continuant</t>
-  </si>
-  <si>
     <t>BCIO:001000</t>
   </si>
   <si>
-    <t>Behaviour change intervention scenario (BCI scenario)</t>
-  </si>
-  <si>
     <t>A process in which a BCI is applied in a given context, including BCI engagement and outcome behaviour.</t>
   </si>
   <si>
     <t>BCIO:028000</t>
   </si>
   <si>
-    <t>Behaviour change intervention scenario plan (BCI scenario plan)</t>
-  </si>
-  <si>
     <t>A plan that is realized in a BCI scenario process.</t>
   </si>
   <si>
     <t>BCIO:009000</t>
   </si>
   <si>
-    <t xml:space="preserve">Behaviour change intervention schedule of delivery (BCI schedule of delivery) </t>
-  </si>
-  <si>
     <t>An attribute of a BCI that involves its temporal organisation.</t>
   </si>
   <si>
@@ -337,9 +217,6 @@
     <t>BCIO:014000</t>
   </si>
   <si>
-    <t>Behaviour change intervention setting (BCI setting)</t>
-  </si>
-  <si>
     <t xml:space="preserve">An aggregate of entities that form the environment in which a BCI is provided. </t>
   </si>
   <si>
@@ -349,63 +226,36 @@
     <t>BCIO:029000</t>
   </si>
   <si>
-    <t>Behaviour change intervention social setting (BCI social setting)</t>
-  </si>
-  <si>
     <t>An aggregate of people with whom a BCI population interacts.</t>
   </si>
   <si>
-    <t>Human population/Continuant</t>
-  </si>
-  <si>
     <t>BCIO:010000</t>
   </si>
   <si>
-    <t>Behaviour change intervention source (BCI source)</t>
-  </si>
-  <si>
     <t>A role played by a person, population or organisation that provides a BCI.</t>
   </si>
   <si>
-    <t xml:space="preserve">Role/Role </t>
-  </si>
-  <si>
     <t>This includes individual people, groups of people, and organisations.</t>
   </si>
   <si>
     <t>BCIO:030000</t>
   </si>
   <si>
-    <t>Behaviour change intervention study investigator (BCI study investigator)</t>
-  </si>
-  <si>
     <t>A role played by a person that contributes substantively to production or reporting of a BCI evaluation study.</t>
   </si>
   <si>
-    <t>Role/Role</t>
-  </si>
-  <si>
     <t xml:space="preserve">What counts as substantively is subject to judgement. The level and nature of the contribution can be defined using the CReDiT taxonomy (https://casrai.org/credit/). </t>
   </si>
   <si>
     <t>BCIO:031000</t>
   </si>
   <si>
-    <t>Behaviour change intervention study sample (BCI study sample)</t>
-  </si>
-  <si>
     <t>A population whose behaviour is studied in a BCI evaluation study.</t>
   </si>
   <si>
-    <t>Human population/Object aggregate</t>
-  </si>
-  <si>
     <t>BCIO:044000</t>
   </si>
   <si>
-    <t>Behaviour change intervention style of delivery (BCI style of delivery)</t>
-  </si>
-  <si>
     <t>An attribute of BCI delivery that encompasses the characteristics of how BCI content is communicated.</t>
   </si>
   <si>
@@ -415,84 +265,48 @@
     <t>BCIO:032000</t>
   </si>
   <si>
-    <t>Behaviour change intervention tailoring (BCI tailoring)</t>
-  </si>
-  <si>
     <t>An attribute of a BCI that relates to selection or modification of the BCI according to attributes of members of the BCI population or BCI context.</t>
   </si>
   <si>
-    <t xml:space="preserve">Process attribute/Process </t>
-  </si>
-  <si>
     <t>It includes static tailoring that is based on characteristics of a member of a BCI population or BCI context at a single point in time and dynamic tailoring that can change as a function of characteristics assessed at multiple time points.</t>
   </si>
   <si>
     <t>BCIO:033000</t>
   </si>
   <si>
-    <t>Behaviour change technique (BCT)</t>
-  </si>
-  <si>
     <t>A planned process that is the smallest part of BCI content that is observable, replicable and on its own has the potential to bring about behaviour change.</t>
   </si>
   <si>
-    <t xml:space="preserve">Planned process (OBI)/Process </t>
-  </si>
-  <si>
     <t>BCIO:002000</t>
   </si>
   <si>
-    <t>Outcome behaviour</t>
-  </si>
-  <si>
     <t>Human behavior that is an intervention outcome.</t>
   </si>
   <si>
-    <t xml:space="preserve">Human behaviour/Process </t>
-  </si>
-  <si>
     <t>BCIO:034000</t>
   </si>
   <si>
-    <t>Population behaviour</t>
-  </si>
-  <si>
     <t>An aggregate of individual human behaviours of members of a population.</t>
   </si>
   <si>
-    <t>Process/Process</t>
-  </si>
-  <si>
     <t>BCIO:035000</t>
   </si>
   <si>
-    <t>Evaluation finding</t>
-  </si>
-  <si>
     <t>A data item that is the output of an intervention evaluation study.</t>
   </si>
   <si>
-    <t xml:space="preserve">Data item (IAO)/Continuant </t>
-  </si>
-  <si>
     <t>Also referred to in definitions as human behaviour or just behaviour.</t>
   </si>
   <si>
     <t>BCIO:036000</t>
   </si>
   <si>
-    <t>Individual human behaviour</t>
-  </si>
-  <si>
     <t xml:space="preserve">Individual human activity that involves co-ordinated contraction of striated muscles controlled by the brain. </t>
   </si>
   <si>
     <t>BCIO:037000</t>
   </si>
   <si>
-    <t>Intervention</t>
-  </si>
-  <si>
     <t>A planned process that has the aim of influencing an outcome.</t>
   </si>
   <si>
@@ -502,21 +316,12 @@
     <t>BCIO:038000</t>
   </si>
   <si>
-    <t>Intervention evaluation study</t>
-  </si>
-  <si>
     <t>A research study that aims to assess attributes of an intervention with regards to their positive or negative value.</t>
   </si>
   <si>
-    <t xml:space="preserve">Research study (SEPIO)/Process </t>
-  </si>
-  <si>
     <t>BCIO:039000</t>
   </si>
   <si>
-    <t>Intervention outcome</t>
-  </si>
-  <si>
     <t>A process that is influenced by an intervention.</t>
   </si>
   <si>
@@ -526,40 +331,247 @@
     <t>BCIO:040000</t>
   </si>
   <si>
-    <t>Individual human activity</t>
-  </si>
-  <si>
     <t>A process that is produced by a person.</t>
   </si>
   <si>
     <t>BCIO:041000</t>
   </si>
   <si>
-    <t>Human population</t>
-  </si>
-  <si>
     <t>An aggregate of people</t>
   </si>
   <si>
     <t>BCIO:042000</t>
   </si>
   <si>
-    <t>Human behaviour</t>
-  </si>
-  <si>
     <t>Individual human behaviour or population behaviour</t>
   </si>
   <si>
     <t>BCIO:043000</t>
   </si>
   <si>
-    <t>Process attribute</t>
-  </si>
-  <si>
     <t>An attribute of a process</t>
   </si>
   <si>
-    <t>Process profile/Process profile</t>
+    <t>behaviour change intervention (BCI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intervention/process </t>
+  </si>
+  <si>
+    <t>behaviour change intervention comparison evaluation study (BCI comparison evaluation study)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention content (BCI content)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">behaviour change intervention evaluation study/process </t>
+  </si>
+  <si>
+    <t>planned process (OBI)/process</t>
+  </si>
+  <si>
+    <t>behaviour change intervention context (BCI context)</t>
+  </si>
+  <si>
+    <t>object aggregate/object aggregate</t>
+  </si>
+  <si>
+    <t>behaviour change intervention delivery (BCI delivery)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention dose (BCI dose)</t>
+  </si>
+  <si>
+    <t>process attribute/process</t>
+  </si>
+  <si>
+    <t>behaviour change intervention effect estimate (BCI effect estimate)</t>
+  </si>
+  <si>
+    <t>BCI evaluation finding/generically dependent continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention engagement (BCI engagement)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">individual human activity/process </t>
+  </si>
+  <si>
+    <t>behaviour change intervention evaluation finding (BCI evaluation finding)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evaluation finding/process </t>
+  </si>
+  <si>
+    <t>behaviour change intervention evaluation report (BCI evaluation report)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report (IAO)/generically dependent continuant </t>
+  </si>
+  <si>
+    <t>behaviour change intervention evaluation study (BCI evaluation study)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intervention evaluation study/process </t>
+  </si>
+  <si>
+    <t>behaviour change intervention evaluation study plan (BCI evaluation study plan)</t>
+  </si>
+  <si>
+    <t>plan (OBI)/generically dependent continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention evaluation study risk of bias or error (BCI study risk of bias or error)</t>
+  </si>
+  <si>
+    <t>information content entity (IAO)/generically dependent continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention mechanism of action (BCI mechanism of action)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">process/process </t>
+  </si>
+  <si>
+    <t>behaviour change intervention mode of delivery (BCI mode of delivery)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention outcome estimate (BCI outcome estimate)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention evaluation finding/generically dependent continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention physical setting (BCI physical setting)</t>
+  </si>
+  <si>
+    <t>environmental system (ENVO)/continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention population (BCI population)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human population/object aggregate </t>
+  </si>
+  <si>
+    <t>behaviour change intervention scenario report (BCI scenario report)</t>
+  </si>
+  <si>
+    <t>report (IAO)/generically dependent continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention scenario (BCI scenario)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention scenario plan (BCI scenario plan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">behaviour change intervention schedule of delivery (BCI schedule of delivery) </t>
+  </si>
+  <si>
+    <t>behaviour change intervention setting (BCI setting)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention social setting (BCI social setting)</t>
+  </si>
+  <si>
+    <t>human population/continuant</t>
+  </si>
+  <si>
+    <t>behaviour change intervention source (BCI source)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role/role </t>
+  </si>
+  <si>
+    <t>behaviour change intervention study investigator (BCI study investigator)</t>
+  </si>
+  <si>
+    <t>role/role</t>
+  </si>
+  <si>
+    <t>behaviour change intervention study sample (BCI study sample)</t>
+  </si>
+  <si>
+    <t>human population/object aggregate</t>
+  </si>
+  <si>
+    <t>behaviour change intervention style of delivery (BCI style of delivery)</t>
+  </si>
+  <si>
+    <t>behaviour change intervention tailoring (BCI tailoring)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">process attribute/process </t>
+  </si>
+  <si>
+    <t>behaviour change technique (BCT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">planned process (OBI)/process </t>
+  </si>
+  <si>
+    <t>outcome behaviour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human behaviour/process </t>
+  </si>
+  <si>
+    <t>population behaviour</t>
+  </si>
+  <si>
+    <t>process/process</t>
+  </si>
+  <si>
+    <t>evaluation finding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data item (IAO)/continuant </t>
+  </si>
+  <si>
+    <t>individual human behaviour</t>
+  </si>
+  <si>
+    <t>intervention</t>
+  </si>
+  <si>
+    <t>intervention evaluation study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">research study (SEPIO)/process </t>
+  </si>
+  <si>
+    <t>intervention outcome</t>
+  </si>
+  <si>
+    <t>individual human activity</t>
+  </si>
+  <si>
+    <t>human population</t>
+  </si>
+  <si>
+    <t>human behaviour</t>
+  </si>
+  <si>
+    <t>process attribute</t>
+  </si>
+  <si>
+    <t>process profile/process profile</t>
+  </si>
+  <si>
+    <t>intervention delivery</t>
+  </si>
+  <si>
+    <t>A process by which intervention content is delivered.</t>
+  </si>
+  <si>
+    <t>An intervention delivery in which the intervention is a behaviour change intervention.</t>
+  </si>
+  <si>
+    <t>('indivdiual human behaviour' or 'population behaviour')</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
   </si>
 </sst>
 </file>
@@ -911,22 +923,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-    <col min="3" max="3" width="79.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" customWidth="1"/>
+    <col min="3" max="3" width="79.1640625" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -958,943 +971,960 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>179</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+        <v>124</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>161</v>
+        <v>98</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>15</v>
+        <v>183</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>176</v>
+        <v>108</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" t="s">
+        <v>180</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change status to published
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
@@ -39,7 +39,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ffe4b5"/>
+        <fgColor rgb="007fffd4"/>
       </patternFill>
     </fill>
     <fill>
@@ -523,10 +523,14 @@
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr"/>
-      <c r="G2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr"/>
@@ -559,10 +563,14 @@
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr"/>
-      <c r="G3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr"/>
@@ -631,10 +639,14 @@
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr"/>
-      <c r="G5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr"/>
@@ -663,10 +675,14 @@
       </c>
       <c r="E6" s="2" t="inlineStr"/>
       <c r="F6" s="2" t="inlineStr"/>
-      <c r="G6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr"/>
@@ -699,10 +715,14 @@
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr"/>
-      <c r="G7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr"/>
@@ -735,10 +755,14 @@
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr"/>
-      <c r="G8" s="2" t="inlineStr"/>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr"/>
@@ -771,10 +795,14 @@
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr"/>
-      <c r="G9" s="2" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr"/>
@@ -803,10 +831,14 @@
       </c>
       <c r="E10" s="2" t="inlineStr"/>
       <c r="F10" s="2" t="inlineStr"/>
-      <c r="G10" s="2" t="inlineStr"/>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr"/>
@@ -839,10 +871,14 @@
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr"/>
-      <c r="G11" s="2" t="inlineStr"/>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I11" s="2" t="inlineStr"/>
@@ -871,10 +907,14 @@
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="2" t="inlineStr"/>
-      <c r="G12" s="2" t="inlineStr"/>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
@@ -903,10 +943,14 @@
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="2" t="inlineStr"/>
-      <c r="G13" s="2" t="inlineStr"/>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
@@ -935,10 +979,14 @@
       </c>
       <c r="E14" s="2" t="inlineStr"/>
       <c r="F14" s="2" t="inlineStr"/>
-      <c r="G14" s="2" t="inlineStr"/>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H14" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I14" s="2" t="inlineStr"/>
@@ -969,12 +1017,12 @@
       <c r="F15" s="2" t="inlineStr"/>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>PS; JH</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I15" s="2" t="inlineStr"/>
@@ -1003,10 +1051,14 @@
       </c>
       <c r="E16" s="2" t="inlineStr"/>
       <c r="F16" s="2" t="inlineStr"/>
-      <c r="G16" s="2" t="inlineStr"/>
+      <c r="G16" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I16" s="2" t="inlineStr"/>
@@ -1039,10 +1091,14 @@
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr"/>
-      <c r="G17" s="2" t="inlineStr"/>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I17" s="2" t="inlineStr"/>
@@ -1071,10 +1127,14 @@
       </c>
       <c r="E18" s="2" t="inlineStr"/>
       <c r="F18" s="2" t="inlineStr"/>
-      <c r="G18" s="2" t="inlineStr"/>
+      <c r="G18" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr"/>
@@ -1103,10 +1163,14 @@
       </c>
       <c r="E19" s="2" t="inlineStr"/>
       <c r="F19" s="2" t="inlineStr"/>
-      <c r="G19" s="2" t="inlineStr"/>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H19" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I19" s="2" t="inlineStr"/>
@@ -1135,10 +1199,14 @@
       </c>
       <c r="E20" s="2" t="inlineStr"/>
       <c r="F20" s="2" t="inlineStr"/>
-      <c r="G20" s="2" t="inlineStr"/>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I20" s="2" t="inlineStr"/>
@@ -1167,10 +1235,14 @@
       </c>
       <c r="E21" s="2" t="inlineStr"/>
       <c r="F21" s="2" t="inlineStr"/>
-      <c r="G21" s="2" t="inlineStr"/>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr"/>
@@ -1199,10 +1271,14 @@
       </c>
       <c r="E22" s="2" t="inlineStr"/>
       <c r="F22" s="2" t="inlineStr"/>
-      <c r="G22" s="2" t="inlineStr"/>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I22" s="2" t="inlineStr"/>
@@ -1235,10 +1311,14 @@
         </is>
       </c>
       <c r="F23" s="2" t="inlineStr"/>
-      <c r="G23" s="2" t="inlineStr"/>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H23" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I23" s="2" t="inlineStr"/>
@@ -1271,10 +1351,14 @@
         </is>
       </c>
       <c r="F24" s="2" t="inlineStr"/>
-      <c r="G24" s="2" t="inlineStr"/>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H24" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I24" s="2" t="inlineStr"/>
@@ -1303,10 +1387,14 @@
       </c>
       <c r="E25" s="2" t="inlineStr"/>
       <c r="F25" s="2" t="inlineStr"/>
-      <c r="G25" s="2" t="inlineStr"/>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I25" s="2" t="inlineStr"/>
@@ -1339,10 +1427,14 @@
         </is>
       </c>
       <c r="F26" s="2" t="inlineStr"/>
-      <c r="G26" s="2" t="inlineStr"/>
+      <c r="G26" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I26" s="2" t="inlineStr"/>
@@ -1375,10 +1467,14 @@
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr"/>
-      <c r="G27" s="2" t="inlineStr"/>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I27" s="2" t="inlineStr"/>
@@ -1407,10 +1503,14 @@
       </c>
       <c r="E28" s="2" t="inlineStr"/>
       <c r="F28" s="2" t="inlineStr"/>
-      <c r="G28" s="2" t="inlineStr"/>
+      <c r="G28" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H28" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I28" s="2" t="inlineStr"/>
@@ -1443,10 +1543,14 @@
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr"/>
-      <c r="G29" s="2" t="inlineStr"/>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I29" s="2" t="inlineStr"/>
@@ -1479,10 +1583,14 @@
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr"/>
-      <c r="G30" s="2" t="inlineStr"/>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H30" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I30" s="2" t="inlineStr"/>
@@ -1511,10 +1619,14 @@
       </c>
       <c r="E31" s="2" t="inlineStr"/>
       <c r="F31" s="2" t="inlineStr"/>
-      <c r="G31" s="2" t="inlineStr"/>
+      <c r="G31" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H31" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I31" s="2" t="inlineStr"/>
@@ -1543,10 +1655,14 @@
       </c>
       <c r="E32" s="2" t="inlineStr"/>
       <c r="F32" s="2" t="inlineStr"/>
-      <c r="G32" s="2" t="inlineStr"/>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I32" s="2" t="inlineStr"/>
@@ -1607,10 +1723,14 @@
       </c>
       <c r="E34" s="2" t="inlineStr"/>
       <c r="F34" s="2" t="inlineStr"/>
-      <c r="G34" s="2" t="inlineStr"/>
+      <c r="G34" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H34" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I34" s="2" t="inlineStr"/>
@@ -1639,10 +1759,14 @@
       </c>
       <c r="E35" s="2" t="inlineStr"/>
       <c r="F35" s="2" t="inlineStr"/>
-      <c r="G35" s="2" t="inlineStr"/>
+      <c r="G35" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H35" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I35" s="2" t="inlineStr"/>
@@ -1679,10 +1803,14 @@
           <t>human behaviour</t>
         </is>
       </c>
-      <c r="G36" s="2" t="inlineStr"/>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I36" s="2" t="inlineStr"/>
@@ -1715,10 +1843,14 @@
         </is>
       </c>
       <c r="F37" s="2" t="inlineStr"/>
-      <c r="G37" s="2" t="inlineStr"/>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I37" s="2" t="inlineStr"/>
@@ -1811,10 +1943,14 @@
       </c>
       <c r="E40" s="2" t="inlineStr"/>
       <c r="F40" s="2" t="inlineStr"/>
-      <c r="G40" s="2" t="inlineStr"/>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H40" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I40" s="2" t="inlineStr"/>
@@ -1847,10 +1983,14 @@
         </is>
       </c>
       <c r="F41" s="2" t="inlineStr"/>
-      <c r="G41" s="2" t="inlineStr"/>
+      <c r="G41" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I41" s="2" t="inlineStr"/>
@@ -1879,10 +2019,14 @@
       </c>
       <c r="E42" s="2" t="inlineStr"/>
       <c r="F42" s="2" t="inlineStr"/>
-      <c r="G42" s="2" t="inlineStr"/>
+      <c r="G42" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H42" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I42" s="2" t="inlineStr"/>
@@ -1915,10 +2059,14 @@
           <t>human behaviour</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr"/>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I43" s="2" t="inlineStr"/>
@@ -1947,10 +2095,14 @@
       </c>
       <c r="E44" s="2" t="inlineStr"/>
       <c r="F44" s="2" t="inlineStr"/>
-      <c r="G44" s="2" t="inlineStr"/>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>Discussed</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I44" s="2" t="inlineStr"/>

</xml_diff>

<commit_message>
Update Upper level BCIO
Added sub-ontology for two entities
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisazhang/Documents/GitHub/ontologies/Upper Level BCIO/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micas\OneDrive\Documentos\GitHub\ontologies\Upper Level BCIO\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93461DE8-5668-F84B-A7CB-75B15C2A6429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3C8E3D-7D34-4A57-9E07-3EA900A88676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8260" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="249">
   <si>
     <t>ID</t>
   </si>
@@ -1133,18 +1133,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="18.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1233,9 @@
       <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1256,7 +1258,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1277,7 +1279,9 @@
       <c r="H3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1298,7 +1302,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1348,7 +1352,7 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -1394,7 +1398,7 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>55</v>
       </c>
@@ -1440,7 +1444,7 @@
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
@@ -1486,7 +1490,7 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>67</v>
       </c>
@@ -1530,7 +1534,7 @@
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>72</v>
       </c>
@@ -1578,7 +1582,7 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -1624,7 +1628,7 @@
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>83</v>
       </c>
@@ -1670,7 +1674,7 @@
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>89</v>
       </c>
@@ -1714,7 +1718,7 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>94</v>
       </c>
@@ -1760,7 +1764,7 @@
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>101</v>
       </c>
@@ -1804,7 +1808,7 @@
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>105</v>
       </c>
@@ -1848,7 +1852,7 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>110</v>
       </c>
@@ -1892,7 +1896,7 @@
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>114</v>
       </c>
@@ -1936,7 +1940,7 @@
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>119</v>
       </c>
@@ -1980,7 +1984,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>123</v>
       </c>
@@ -2026,7 +2030,7 @@
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>128</v>
       </c>
@@ -2068,7 +2072,7 @@
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>133</v>
       </c>
@@ -2110,7 +2114,7 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>137</v>
       </c>
@@ -2152,7 +2156,7 @@
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>141</v>
       </c>
@@ -2194,7 +2198,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>145</v>
       </c>
@@ -2236,7 +2240,7 @@
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>149</v>
       </c>
@@ -2280,7 +2284,7 @@
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>153</v>
       </c>
@@ -2324,7 +2328,7 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>158</v>
       </c>
@@ -2366,7 +2370,7 @@
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>162</v>
       </c>
@@ -2410,7 +2414,7 @@
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>168</v>
       </c>
@@ -2454,7 +2458,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>173</v>
       </c>
@@ -2496,7 +2500,7 @@
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>177</v>
       </c>
@@ -2540,7 +2544,7 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>181</v>
       </c>
@@ -2588,7 +2592,7 @@
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>187</v>
       </c>
@@ -2630,7 +2634,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>191</v>
       </c>
@@ -2672,7 +2676,7 @@
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>196</v>
       </c>
@@ -2714,7 +2718,7 @@
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>200</v>
       </c>
@@ -2754,7 +2758,7 @@
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>203</v>
       </c>
@@ -2792,7 +2796,7 @@
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>208</v>
       </c>
@@ -2832,7 +2836,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>210</v>
       </c>
@@ -2872,7 +2876,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>212</v>
       </c>
@@ -2916,7 +2920,7 @@
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>215</v>
       </c>
@@ -2958,7 +2962,7 @@
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>218</v>
       </c>
@@ -2998,7 +3002,7 @@
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>220</v>
       </c>
@@ -3038,7 +3042,7 @@
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>221</v>
       </c>
@@ -3078,7 +3082,7 @@
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>224</v>
       </c>
@@ -3120,7 +3124,7 @@
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>228</v>
       </c>
@@ -3160,7 +3164,7 @@
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>231</v>
       </c>
@@ -3202,7 +3206,7 @@
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>234</v>
       </c>

</xml_diff>